<commit_message>
"Final revisions and testing completed."
</commit_message>
<xml_diff>
--- a/eterno_data.xlsx
+++ b/eterno_data.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,6 +510,31 @@
       <c r="E3" t="inlineStr">
         <is>
           <t>2025-11-05 23:21:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>kaizen</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>boarratjabol@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>customer</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:59:58</t>
         </is>
       </c>
     </row>
@@ -524,7 +549,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -580,15 +605,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Eterno Shirt</t>
+          <t>Eterno Void</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>500</v>
+        <v>599</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -597,7 +622,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://scontent.fmnl33-2.fna.fbcdn.net/v/t39.30808-6/504252726_122141015126602772_536880939443070759_n.jpg?_nc_cat=104&amp;ccb=1-7&amp;_nc_sid=833d8c&amp;_nc_eui2=AeFAXFAPxLaUp8be64JV-o_kTzezJOlsE6pPN7Mk6WwTqu54</t>
+          <t>https://i.ibb.co/sd7crdHV/468614642-122110597646602772-5741305816202520031-n.jpg</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -620,7 +645,7 @@
         <v>799</v>
       </c>
       <c r="E3" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -629,12 +654,396 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://scontent.fmnl4-2.fna.fbcdn.net/v/t39.30808-6/504703845_122141015084602772_3956461215141399652_n.jpg?_nc_cat=101&amp;ccb=1-7&amp;_nc_sid=833d8c&amp;_nc_eui2=AeHv6WNx7LBx46VCvlHlNWDBVZpztma7UA9VmnO2ZrtQD7oA</t>
+          <t>https://i.ibb.co/23s110xr/504703845-122141015084602772-3956461215141399652-n.jpg</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>2025-11-08 06:47:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Eterno Outlaw</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>1199</v>
+      </c>
+      <c r="E4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Jackets</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/4RvHGQnL/504812987-122140885244602772-6478208165150186098-n.jpg</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:17:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Eterno Saint</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>1399</v>
+      </c>
+      <c r="E5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Jackets</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/fz1y42b0/545423967-122152407638602772-4284048291396969698-n.jpg</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:17:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Eterno Pulse</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>499</v>
+      </c>
+      <c r="E6" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Shirts</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/GQVDzrxf/Screenshot-2025-11-09-212227.png</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:33:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Eterno Sanctum</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>499</v>
+      </c>
+      <c r="E7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Shirts</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/BHDjYFJT/504252726-122141015126602772-536880939443070759-n.jpg</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:34:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Eterno Eclipse</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>4999</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Outerwear</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/27PxvGqV/image.jpg</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:49:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Eterno Abyss</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>4599</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Outerwear</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/356xp46C/Screenshot-2025-11-09-214504.png</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:50:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Eterno Drift</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>3999</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Outerwear</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/kV3YC222/Screenshot-2025-11-09-214421.png</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:51:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Eterno Ethos</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>1999</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Jackets</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/HcTcqJD/Screenshot-2025-11-09-214534.png</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:52:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Bonest Gatti</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="n">
+        <v>25799</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Accessories</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/jvqykhMB/Screenshot-2025-11-09-213836.png</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:53:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Bonest Gatti</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>15999</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Accessories</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/DPXp1GYv/Screenshot-2025-11-09-213909.png</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:54:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Bonest Gatti</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>26789</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Accessories</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/GvXy6tG1/Screenshot-2025-11-09-214106.png</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:55:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Bonest Gatti</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>24509</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Accessories</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/dsVq1kRp/Screenshot-2025-11-09-214036.png</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2025-11-09 13:55:51</t>
         </is>
       </c>
     </row>
@@ -649,7 +1058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -764,6 +1173,74 @@
       <c r="H3" t="inlineStr">
         <is>
           <t>2025-11-08 07:12:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>voucher</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[{"product_id": 2, "name": "Eterno Grace", "price": 799, "quantity": 2, "stock": 19}, {"product_id": 1, "name": "Eterno Shirt", "price": 500, "quantity": 1, "stock": 5}]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-11-08 07:25:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>20639.2</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>senior</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>5159.8</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>[{"product_id": 11, "name": "Bonest Gatti", "price": 25799, "quantity": 1, "stock": 4}]</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2025-11-09 14:18:29</t>
         </is>
       </c>
     </row>
@@ -778,7 +1255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1004,6 +1481,318 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G5" t="n">
+        <v>55</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1354</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>credit_card</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>[{"product_id": 2, "product_name": "Eterno Grace", "quantity": 1, "price": 799.0}, {"product_id": 1, "product_name": "Eterno Shirt", "quantity": 1, "price": 500.0}]</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2025-11-09 12:09:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>500</v>
+      </c>
+      <c r="G6" t="n">
+        <v>167</v>
+      </c>
+      <c r="H6" t="n">
+        <v>567</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>paypal</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>[{"product_id": 1, "product_name": "Eterno Shirt", "quantity": 1, "price": 500.0}]</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2025-11-09 12:12:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>799</v>
+      </c>
+      <c r="G7" t="n">
+        <v>61</v>
+      </c>
+      <c r="H7" t="n">
+        <v>760</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>gcash</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>[{"product_id": 2, "product_name": "Eterno Grace", "quantity": 1, "price": 799.0}]</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2025-11-09 12:12:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>egg street egg city egg municipal</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>500</v>
+      </c>
+      <c r="G8" t="n">
+        <v>168</v>
+      </c>
+      <c r="H8" t="n">
+        <v>668</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>cod</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>[{"product_id": 1, "product_name": "Eterno Shirt", "quantity": 1, "price": 500.0}]</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2025-11-09 12:13:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>kaizen</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>boarratjabol@gmail.com</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>4599</v>
+      </c>
+      <c r="G9" t="n">
+        <v>76</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4575</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>credit_card</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>[{"product_id": 8, "product_name": "Eterno Abyss", "quantity": 1, "price": 4599.0}]</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2025-11-09 14:01:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>kaizen</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>boarratjabol@gmail.com</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>25799</v>
+      </c>
+      <c r="G10" t="n">
+        <v>50</v>
+      </c>
+      <c r="H10" t="n">
+        <v>25749</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>credit_card</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>[{"product_id": 11, "product_name": "Bonest Gatti", "quantity": 1, "price": 25799.0}]</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2025-11-09 14:16:10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
"Separated admin routes and templates from main application structure"
</commit_message>
<xml_diff>
--- a/eterno_data.xlsx
+++ b/eterno_data.xlsx
@@ -645,7 +645,7 @@
         <v>799</v>
       </c>
       <c r="E3" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -869,7 +869,7 @@
         <v>3999</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1058,7 +1058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1241,6 +1241,40 @@
       <c r="H5" t="inlineStr">
         <is>
           <t>2025-11-09 14:18:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1498</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>voucher</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>100</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>[{"product_id": 2, "name": "Eterno Grace", "price": 799, "quantity": 2, "stock": 15}]</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025-11-09 15:37:44</t>
         </is>
       </c>
     </row>
@@ -1255,7 +1289,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1793,6 +1827,58 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>kaizen</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>boarratjabol@gmail.com</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>blk 32 lot 12, Paloma Street, Garden of Edem, Greece, Europe</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>3999</v>
+      </c>
+      <c r="G11" t="n">
+        <v>83</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3982</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>cod</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>[{"product_id": 9, "product_name": "Eterno Drift", "quantity": 1, "price": 3999.0}]</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>2025-11-09 15:36:22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
"Final touches to static assets and templates"
</commit_message>
<xml_diff>
--- a/eterno_data.xlsx
+++ b/eterno_data.xlsx
@@ -613,7 +613,7 @@
         <v>599</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1289,7 +1289,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1879,6 +1879,58 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>kaizen</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>boarratjabol@gmail.com</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>599</v>
+      </c>
+      <c r="G12" t="n">
+        <v>77</v>
+      </c>
+      <c r="H12" t="n">
+        <v>676</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>credit_card</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>[{"product_id": 1, "product_name": "Eterno Void", "quantity": 1, "price": 599.0}]</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2025-11-10 02:14:24</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
"Admin control updates and customer enhancements"
</commit_message>
<xml_diff>
--- a/eterno_data.xlsx
+++ b/eterno_data.xlsx
@@ -484,7 +484,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-11-02 05:08:59</t>
+          <t>2025-11-02 13:08:59 SGT</t>
         </is>
       </c>
     </row>
@@ -509,7 +509,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-11-05 23:21:17</t>
+          <t>2025-11-06 07:21:17 SGT</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-11-09 13:59:58</t>
+          <t>2025-11-09 21:59:58 SGT</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-11-10 04:35:47</t>
+          <t>2025-11-10 12:35:47 SGT</t>
         </is>
       </c>
     </row>
@@ -652,7 +652,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-11-05 23:19:36</t>
+          <t>2025-11-06 07:19:36 SGT</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
         <v>799</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -684,7 +684,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-11-08 06:47:45</t>
+          <t>2025-11-08 14:47:45 SGT</t>
         </is>
       </c>
     </row>
@@ -702,7 +702,7 @@
         <v>1199</v>
       </c>
       <c r="E4" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -716,7 +716,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-11-09 13:17:33</t>
+          <t>2025-11-09 21:17:33 SGT</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
         <v>1399</v>
       </c>
       <c r="E5" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -748,7 +748,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-11-09 13:17:53</t>
+          <t>2025-11-09 21:17:53 SGT</t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-11-09 13:33:38</t>
+          <t>2025-11-09 21:33:38 SGT</t>
         </is>
       </c>
     </row>
@@ -812,7 +812,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-11-09 13:34:32</t>
+          <t>2025-11-09 21:34:32 SGT</t>
         </is>
       </c>
     </row>
@@ -844,7 +844,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-11-09 13:49:55</t>
+          <t>2025-11-09 21:49:55 SGT</t>
         </is>
       </c>
     </row>
@@ -862,7 +862,7 @@
         <v>4599</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -876,7 +876,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-11-09 13:50:42</t>
+          <t>2025-11-09 21:50:42 SGT</t>
         </is>
       </c>
     </row>
@@ -908,7 +908,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-11-09 13:51:23</t>
+          <t>2025-11-09 21:51:23 SGT</t>
         </is>
       </c>
     </row>
@@ -940,7 +940,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-11-09 13:52:04</t>
+          <t>2025-11-09 21:52:04 SGT</t>
         </is>
       </c>
     </row>
@@ -972,7 +972,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-11-09 13:53:39</t>
+          <t>2025-11-09 21:53:39 SGT</t>
         </is>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-11-09 13:54:20</t>
+          <t>2025-11-09 21:54:20 SGT</t>
         </is>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-11-09 13:55:09</t>
+          <t>2025-11-09 21:55:09 SGT</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-11-09 13:55:51</t>
+          <t>2025-11-09 21:55:51 SGT</t>
         </is>
       </c>
     </row>
@@ -1083,7 +1083,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-11-05 23:19:59</t>
+          <t>2025-11-06 07:19:59 SGT</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-11-08 07:12:07</t>
+          <t>2025-11-08 15:12:07 SGT</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-11-08 07:25:20</t>
+          <t>2025-11-08 15:25:20 SGT</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-11-09 14:18:29</t>
+          <t>2025-11-09 22:18:29 SGT</t>
         </is>
       </c>
     </row>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-11-09 15:37:44</t>
+          <t>2025-11-09 23:37:44 SGT</t>
         </is>
       </c>
     </row>
@@ -1333,7 +1333,177 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-11-10 04:40:56</t>
+          <t>2025-11-10 12:40:56 SGT</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1399</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>[{"product_id": 4, "name": "Eterno Saint", "price": 1399, "quantity": 1, "stock": 15}]</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2025-11-12 17:36:05 SGT</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1399</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[{"product_id": 4, "name": "Eterno Saint", "price": 1399, "quantity": 1, "stock": 15}]</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2025-11-12 17:36:05 SGT</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1399</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>[{"product_id": 4, "name": "Eterno Saint", "price": 1399, "quantity": 1, "stock": 15}]</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2025-11-12 17:36:05 SGT</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1399</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>[{"product_id": 4, "name": "Eterno Saint", "price": 1399, "quantity": 1, "stock": 15}]</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2025-11-12 17:36:05 SGT</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1199</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>[{"product_id": 3, "name": "Eterno Outlaw", "price": 1199, "quantity": 1, "stock": 18}]</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2025-11-12 17:47:37 SGT</t>
         </is>
       </c>
     </row>
@@ -1348,7 +1518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1466,7 +1636,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-11-08 06:15:10</t>
+          <t>2025-11-08 14:15:10 SGT</t>
         </is>
       </c>
     </row>
@@ -1518,7 +1688,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-11-08 06:15:36</t>
+          <t>2025-11-08 14:15:36 SGT</t>
         </is>
       </c>
     </row>
@@ -1570,7 +1740,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-11-08 07:10:04</t>
+          <t>2025-11-08 15:10:04 SGT</t>
         </is>
       </c>
     </row>
@@ -1622,7 +1792,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-11-09 12:09:55</t>
+          <t>2025-11-09 20:09:55 SGT</t>
         </is>
       </c>
     </row>
@@ -1674,7 +1844,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-11-09 12:12:14</t>
+          <t>2025-11-09 20:12:14 SGT</t>
         </is>
       </c>
     </row>
@@ -1726,7 +1896,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2025-11-09 12:12:59</t>
+          <t>2025-11-09 20:12:59 SGT</t>
         </is>
       </c>
     </row>
@@ -1778,7 +1948,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2025-11-09 12:13:27</t>
+          <t>2025-11-09 20:13:27 SGT</t>
         </is>
       </c>
     </row>
@@ -1830,7 +2000,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2025-11-09 14:01:41</t>
+          <t>2025-11-09 22:01:41 SGT</t>
         </is>
       </c>
     </row>
@@ -1882,7 +2052,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2025-11-09 14:16:10</t>
+          <t>2025-11-09 22:16:10 SGT</t>
         </is>
       </c>
     </row>
@@ -1934,7 +2104,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2025-11-09 15:36:22</t>
+          <t>2025-11-09 23:36:22 SGT</t>
         </is>
       </c>
     </row>
@@ -1986,7 +2156,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2025-11-10 02:14:24</t>
+          <t>2025-11-10 10:14:24 SGT</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2208,117 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2025-11-10 04:37:35</t>
+          <t>2025-11-10 12:37:35 SGT</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>kaizen</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>boarratjabol@gmail.com</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>123123123</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>799</v>
+      </c>
+      <c r="G14" t="n">
+        <v>65</v>
+      </c>
+      <c r="H14" t="n">
+        <v>864</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>credit_card</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>[{"product_id": 2, "product_name": "Eterno Grace", "quantity": 1, "price": 799.0}]</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2025-11-12 17:38:40 SGT</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>kaizen</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>boarratjabol@gmail.com</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Address 1:
+Building Number: 56
+Street Name: Rue Drummond
+Street Address: Ritz-Carlton Montreal
+State: Quebec
+City: Montreal
+Post Code: H3G 1Y9</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>4599</v>
+      </c>
+      <c r="G15" t="n">
+        <v>61</v>
+      </c>
+      <c r="H15" t="n">
+        <v>4660</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>gcash</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>[{"product_id": 8, "product_name": "Eterno Abyss", "quantity": 1, "price": 4599.0}]</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>2025-11-12 17:49:27 SGT</t>
         </is>
       </c>
     </row>

</xml_diff>